<commit_message>
logged time as well as listed tasks
</commit_message>
<xml_diff>
--- a/Time Tracking/time_tracker_horia.xlsx
+++ b/Time Tracking/time_tracker_horia.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D39FFBA-D160-4BC0-B82C-AFD558BD6D76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4589B3-0DE0-4045-81D2-4B2AF0C778A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="time log" sheetId="1" r:id="rId1"/>
+    <sheet name="tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="useful links" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -63,13 +65,76 @@
   </si>
   <si>
     <t>integrating control scheme on board</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>design controller in simulink</t>
+  </si>
+  <si>
+    <t>get parts</t>
+  </si>
+  <si>
+    <t>solder wires to motors</t>
+  </si>
+  <si>
+    <t>read data from imu on kl25z</t>
+  </si>
+  <si>
+    <t>implement control law to control motors with imu input</t>
+  </si>
+  <si>
+    <t>assemble everything</t>
+  </si>
+  <si>
+    <t>implement wireless connectivity and control</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>connect wires to motor shield</t>
+  </si>
+  <si>
+    <t>connect motor shield to kl25z and motor battery</t>
+  </si>
+  <si>
+    <t>solder pins to kl25z for motor function</t>
+  </si>
+  <si>
+    <t>solder pins to kl25z for imu function</t>
+  </si>
+  <si>
+    <t>https://learn.sparkfun.com/tutorials/</t>
+  </si>
+  <si>
+    <t>http://ozzmaker.com/berryimu/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3230nCz3XQA</t>
+  </si>
+  <si>
+    <t>solder header pins to board</t>
+  </si>
+  <si>
+    <t>useful info I2c etc</t>
+  </si>
+  <si>
+    <t>imu to board</t>
+  </si>
+  <si>
+    <t>https://maker.pro/arduino/tutorial/how-to-interface-arduino-and-the-mpu-6050-sensor</t>
+  </si>
+  <si>
+    <t>https://www.intorobotics.com/accelerometer-gyroscope-and-imu-sensors-tutorials/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +150,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,10 +188,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -124,8 +210,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:I11"/>
+  <dimension ref="D4:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,8 +671,204 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="E12" s="5">
+        <v>43382</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="E13" s="5">
+        <v>43383</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="E14" s="5">
+        <v>43384</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="E15" s="5">
+        <v>43394</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="6">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C469A314-0405-4674-BCA9-CB5BFF9D0BAF}">
+  <dimension ref="C3:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="10">
+        <v>43394</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C15" s="10">
+        <v>43431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532E22B-8EBC-49D5-AE28-724217C21C9A}">
+  <dimension ref="D4:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="75.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{40523B81-8462-4BF7-B3F4-FF3D4F588449}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{8D0D5F30-4A7C-4D21-86C1-4007C5FE2DEB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated time and added kl25z files
</commit_message>
<xml_diff>
--- a/Time Tracking/time_tracker_horia.xlsx
+++ b/Time Tracking/time_tracker_horia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71250256-9CA0-441D-9A19-0A48D272D300}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858B1E3D-61F8-44F1-A2D6-23B1C8CA9C2B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="1" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="2" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
   <sheets>
     <sheet name="time log" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>get imu slave adress</t>
+  </si>
+  <si>
+    <t>https://os.mbed.com/platforms/KL25Z/</t>
+  </si>
+  <si>
+    <t>KL25Z info</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:I18"/>
+  <dimension ref="D4:I20"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,6 +763,28 @@
         <v>23</v>
       </c>
     </row>
+    <row r="19" spans="5:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E19" s="5">
+        <v>43396</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="E20" s="5">
+        <v>43397</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -767,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C469A314-0405-4674-BCA9-CB5BFF9D0BAF}">
   <dimension ref="C3:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,10 +891,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532E22B-8EBC-49D5-AE28-724217C21C9A}">
-  <dimension ref="D4:E10"/>
+  <dimension ref="D4:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,6 +952,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{40523B81-8462-4BF7-B3F4-FF3D4F588449}"/>

</xml_diff>

<commit_message>
updated time and added doc for motor driver L9110S
</commit_message>
<xml_diff>
--- a/Time Tracking/time_tracker_horia.xlsx
+++ b/Time Tracking/time_tracker_horia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858B1E3D-61F8-44F1-A2D6-23B1C8CA9C2B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C9CC75-6A68-4D11-8850-1C779D8A5D67}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="2" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>KL25Z info</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=M9lZ5Qy5S2s</t>
+  </si>
+  <si>
+    <t>i2c interface, arduino mpu6050</t>
+  </si>
+  <si>
+    <t>read docs &amp; read data from imu on kl25z</t>
+  </si>
+  <si>
+    <t>https://www.instructables.com/id/Arduino-Nano-Control-Brushelss-DC-Motor-With-L9110/</t>
+  </si>
+  <si>
+    <t>connect motor controller (test) to board</t>
   </si>
 </sst>
 </file>
@@ -560,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:I20"/>
+  <dimension ref="D4:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,6 +800,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="21" spans="5:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E21" s="5">
+        <v>43398</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="E22" s="5">
+        <v>43402</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -796,7 +833,7 @@
   <dimension ref="C3:D17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,15 +928,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532E22B-8EBC-49D5-AE28-724217C21C9A}">
-  <dimension ref="D4:E11"/>
+  <dimension ref="D4:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="75.54296875" customWidth="1"/>
+    <col min="4" max="4" width="77.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:5" x14ac:dyDescent="0.35">
@@ -958,6 +995,22 @@
       </c>
       <c r="E11" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added spec for new motor controller and updated time
</commit_message>
<xml_diff>
--- a/Time Tracking/time_tracker_horia.xlsx
+++ b/Time Tracking/time_tracker_horia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF6ACD0-D05C-4622-9985-892321414028}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98145AB-109C-40A2-8F5A-EBCD2987707B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="2" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
   <sheets>
     <sheet name="time log" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>https://visualgdb.com/tutorials/arm/kinetis/kl25z-rgb-led/</t>
+  </si>
+  <si>
+    <t>integrate functions</t>
+  </si>
+  <si>
+    <t>https://www.instructables.com/id/How-to-use-the-L298-Motor-Driver-Module-Arduino-Tu/</t>
+  </si>
+  <si>
+    <t>https://howtomechatronics.com/tutorials/arduino/arduino-dc-motor-control-tutorial-l298n-pwm-h-bridge/</t>
   </si>
 </sst>
 </file>
@@ -587,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:I28"/>
+  <dimension ref="D4:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,6 +907,28 @@
       </c>
       <c r="I28" s="6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="E29" s="5">
+        <v>43412</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="E30" s="5">
+        <v>43413</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1006,15 +1037,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532E22B-8EBC-49D5-AE28-724217C21C9A}">
-  <dimension ref="D4:E15"/>
+  <dimension ref="D4:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="77.81640625" customWidth="1"/>
+    <col min="4" max="4" width="91.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:5" x14ac:dyDescent="0.35">
@@ -1102,6 +1133,16 @@
     <row r="15" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified project report v1 and updated time spent
</commit_message>
<xml_diff>
--- a/Time Tracking/time_tracker_horia.xlsx
+++ b/Time Tracking/time_tracker_horia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horia\Documents\COEN-6711\Time Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98145AB-109C-40A2-8F5A-EBCD2987707B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F24DB4-B9EC-41B5-B50C-8764CEF3DE93}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" activeTab="2" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{4C9BB474-D0B4-4730-BD29-1D91A56A57B3}"/>
   </bookViews>
   <sheets>
     <sheet name="time log" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -188,6 +189,9 @@
   </si>
   <si>
     <t>https://howtomechatronics.com/tutorials/arduino/arduino-dc-motor-control-tutorial-l298n-pwm-h-bridge/</t>
+  </si>
+  <si>
+    <t>from 11 to 27 Nov</t>
   </si>
 </sst>
 </file>
@@ -596,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876DE979-97A5-4445-B08E-324A54DC235E}">
-  <dimension ref="D4:I30"/>
+  <dimension ref="D4:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -929,6 +933,31 @@
       </c>
       <c r="I30" s="6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="E31" s="5">
+        <v>43414</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="5:9" x14ac:dyDescent="0.35">
+      <c r="E32" s="5">
+        <v>43415</v>
+      </c>
+      <c r="I32" s="6">
+        <f>(27-11)*2</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1039,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1532E22B-8EBC-49D5-AE28-724217C21C9A}">
   <dimension ref="D4:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>